<commit_message>
Use matplotlib to draw figures
</commit_message>
<xml_diff>
--- a/benchmark/macro/result/results.xlsx
+++ b/benchmark/macro/result/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lwyeluo/Workspaces/lab-project/browser/tim-evaluate/benchmark/macro/result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58484C2B-0BAF-1045-B222-65AF8052410C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C365DBDA-D788-3042-8463-BE0428A24B33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FCP-FMP" sheetId="11" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>AVERAGE</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>stanford (crypto)</t>
+  </si>
+  <si>
+    <t>AVERAGE exclude youtube</t>
   </si>
 </sst>
 </file>
@@ -3287,16 +3290,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>77439</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>635001</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>29429</xdr:rowOff>
+      <xdr:rowOff>168820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>46463</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>604025</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>139391</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3664,10 +3667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F524BED2-3A0E-DC44-B2FB-C43862FE7394}">
-  <dimension ref="A1:V184"/>
+  <dimension ref="A1:W184"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="82" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="82" zoomScaleNormal="179" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4540,7 +4543,7 @@
         <v>1920.3417249998954</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B17">
         <v>15</v>
       </c>
@@ -4577,7 +4580,7 @@
         <v>4991.3226500001683</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B18">
         <v>16</v>
       </c>
@@ -4614,7 +4617,7 @@
         <v>5191.6772999979539</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B19">
         <v>17</v>
       </c>
@@ -4651,7 +4654,7 @@
         <v>9676.6162999999542</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B20">
         <v>18</v>
       </c>
@@ -4680,7 +4683,7 @@
         <v>935.02249999716798</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B21">
         <v>19</v>
       </c>
@@ -4709,7 +4712,7 @@
         <v>748.16950000077395</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B22">
         <v>20</v>
       </c>
@@ -4738,7 +4741,7 @@
         <v>739.87649999931398</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -4770,7 +4773,7 @@
         <v>1182.8380000013799</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B24">
         <v>2</v>
       </c>
@@ -4799,7 +4802,7 @@
         <v>913.07999999821095</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B25">
         <v>3</v>
       </c>
@@ -4828,7 +4831,7 @@
         <v>860.97249999828603</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B26">
         <v>4</v>
       </c>
@@ -4859,8 +4862,11 @@
       <c r="V26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="W26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B27">
         <v>5</v>
       </c>
@@ -4932,7 +4938,7 @@
         <v>1.0269451829728569</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B28">
         <v>6</v>
       </c>
@@ -5000,8 +5006,12 @@
         <f>AVERAGE(N28:U28)</f>
         <v>1.0292500105759319</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="W28">
+        <f>(N28+SUM(P28:U28))/7</f>
+        <v>1.0336826577058975</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B29">
         <v>7</v>
       </c>
@@ -5069,8 +5079,12 @@
         <f>AVERAGE(N29:U29)</f>
         <v>1.142065284176792</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="W29">
+        <f>(N29+SUM(P29:U29))/7</f>
+        <v>1.0282620684153823</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B30">
         <v>8</v>
       </c>
@@ -5139,7 +5153,7 @@
         <v>0.96280567097494829</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B31">
         <v>9</v>
       </c>
@@ -5208,7 +5222,7 @@
         <v>0.96427938494781107</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B32">
         <v>10</v>
       </c>
@@ -9665,6 +9679,7 @@
     <hyperlink ref="P2" r:id="rId3" display="www.facebook.com" xr:uid="{4580EBDD-838B-104E-901F-649E251C231E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId4"/>
 </worksheet>
 </file>
@@ -9673,8 +9688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF6D407-A230-3D40-B23A-D945B9CC244C}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>